<commit_message>
Added data for 2 new cities.
</commit_message>
<xml_diff>
--- a/data/new_bird_data.xlsx
+++ b/data/new_bird_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\informatics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2089433D-7714-4007-A8A1-6C826BFA0279}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86A5FC6E-BC0D-4A86-BE94-3F52C541E7C8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17532" windowHeight="5628" xr2:uid="{21B9B352-32BF-48C2-B6AD-33649A01F476}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="41">
   <si>
     <t>elevation</t>
   </si>
@@ -142,13 +142,19 @@
   </si>
   <si>
     <t>Brasilia</t>
+  </si>
+  <si>
+    <t>Salvador</t>
+  </si>
+  <si>
+    <t>Fortaleza</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -159,6 +165,13 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
       <name val="Calibri Light"/>
       <family val="2"/>
       <scheme val="major"/>
@@ -184,9 +197,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -501,10 +515,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74F1CFA0-0373-49B7-A337-54D1C6455447}">
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1101,63 +1115,103 @@
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A32" s="1" t="s">
+      <c r="A32" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B32" s="1">
+      <c r="B32" s="2">
         <v>1172</v>
       </c>
-      <c r="C32" s="1">
+      <c r="C32" s="2">
         <v>6</v>
       </c>
-      <c r="D32" s="1">
+      <c r="D32" s="2">
         <v>5</v>
       </c>
-      <c r="E32" s="1">
-        <v>3</v>
-      </c>
-      <c r="F32" s="1">
-        <v>1</v>
+      <c r="E32" s="2">
+        <v>13</v>
+      </c>
+      <c r="F32" s="2">
+        <v>4</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A33" s="1" t="s">
+      <c r="A33" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B33" s="1">
+      <c r="B33" s="2">
         <v>50</v>
       </c>
-      <c r="C33" s="1">
+      <c r="C33" s="2">
         <v>6</v>
       </c>
-      <c r="D33" s="1">
+      <c r="D33" s="2">
         <v>4</v>
       </c>
-      <c r="E33" s="1">
+      <c r="E33" s="2">
+        <v>12</v>
+      </c>
+      <c r="F33" s="2">
         <v>2</v>
       </c>
-      <c r="F33" s="1">
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B34" s="2">
+        <v>760</v>
+      </c>
+      <c r="C34" s="2">
+        <v>6</v>
+      </c>
+      <c r="D34" s="2">
+        <v>3</v>
+      </c>
+      <c r="E34" s="2">
+        <v>9</v>
+      </c>
+      <c r="F34" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B35" s="2">
+        <v>10</v>
+      </c>
+      <c r="C35" s="2">
+        <v>6</v>
+      </c>
+      <c r="D35" s="2">
+        <v>7</v>
+      </c>
+      <c r="E35" s="2">
+        <v>15</v>
+      </c>
+      <c r="F35" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B36" s="2">
+        <v>21</v>
+      </c>
+      <c r="C36" s="2">
+        <v>6</v>
+      </c>
+      <c r="D36" s="2">
+        <v>10</v>
+      </c>
+      <c r="E36" s="2">
+        <v>11</v>
+      </c>
+      <c r="F36" s="2">
         <v>2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A34" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B34" s="1">
-        <v>760</v>
-      </c>
-      <c r="C34" s="1">
-        <v>6</v>
-      </c>
-      <c r="D34" s="1">
-        <v>3</v>
-      </c>
-      <c r="E34" s="1">
-        <v>4</v>
-      </c>
-      <c r="F34" s="1">
-        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>